<commit_message>
Atualização automática de IGREJINHA.xlsx
</commit_message>
<xml_diff>
--- a/IGREJINHA.xlsx
+++ b/IGREJINHA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B5080BF7-21DE-4D51-9D0E-7B578AA8B3E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{360B2D85-E1CD-42C9-9A9A-938FC882715A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1105,7 +1105,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -1165,36 +1165,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1233,14 +1209,9 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1279,7 +1250,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{6D756080-7168-4399-92C6-7FED59C6F64C}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{C2D15F1D-1071-46A0-9D1C-3FF08EE4EDBF}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1309,10 +1280,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4FAD5CA1-32C1-4E3A-B4CE-43E13737CC2C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2D83CD80-4258-4371-B8F9-E93F29799C81}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1350,7 +1321,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2C5B5A72-3493-4EC3-A527-B4C872E02849}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E7DB3608-58FB-4B4D-8A26-21C989C629F0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1413,7 +1384,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2212CEFE-EB9D-44CC-BFE5-4F8219DAA2AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEE37DC7-5CEB-476B-882C-B6C4D3FB8449}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1432,7 +1403,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{76D5A051-DE50-0EDC-C41B-2432D68283D2}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C5231D0-8EB1-7CCD-B093-55ED88FDD349}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1481,7 +1452,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C16A634-F6E4-D60C-A255-B1C32962DCEF}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0F76E615-5500-FE0D-1DA9-686576189D83}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1500,7 +1471,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{81D00F1D-672A-2EB8-9DC5-76A5BB9DDABF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F3354058-4ABB-7FBC-4928-F351BB05C48D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1531,7 +1502,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D710AF73-1880-1202-3413-61135AF1F261}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CEBE518-D120-E06F-5B65-E1312B7B00AC}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1562,7 +1533,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF5F2342-B253-119E-D72B-5112D12F01E3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{037A4487-B516-1F49-85B3-E4313CA08E04}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1605,7 +1576,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B1F602B-6A96-4993-A099-0477209854E5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62F35209-0846-4D39-9537-203E28649ABC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1643,7 +1614,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA55C0EC-D36B-42FE-92B6-890DA88E4C5B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A4F2E04-0ADF-4ED0-AC5A-692BBE2C58DA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1686,7 +1657,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{523787F4-259B-4E8E-B9B9-5E79F107C055}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{239D3555-52FC-4B9C-8671-5DFC0D47CFF9}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1999,7 +1970,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A0B032-58F2-4723-A790-AE9C555EDF21}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{978EE221-562A-4A50-97EE-7254A8FFE686}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -2011,98 +1982,98 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="5" width="12.5703125" style="36"/>
-    <col min="6" max="6" width="2" style="36" customWidth="1"/>
-    <col min="7" max="16" width="13.42578125" style="36" customWidth="1"/>
-    <col min="17" max="16384" width="12.5703125" style="36"/>
+    <col min="1" max="5" width="12.5703125" style="33"/>
+    <col min="6" max="6" width="2" style="33" customWidth="1"/>
+    <col min="7" max="16" width="13.42578125" style="33" customWidth="1"/>
+    <col min="17" max="16384" width="12.5703125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F1" s="35"/>
+      <c r="F1" s="32"/>
     </row>
     <row r="2" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F2" s="35"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F3" s="35"/>
+      <c r="F3" s="32"/>
     </row>
     <row r="4" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F4" s="35"/>
+      <c r="F4" s="32"/>
     </row>
     <row r="5" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F5" s="35"/>
+      <c r="F5" s="32"/>
     </row>
     <row r="6" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F6" s="35"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F7" s="35"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F8" s="35"/>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F9" s="35"/>
+      <c r="F9" s="32"/>
     </row>
     <row r="10" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F10" s="35"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F11" s="35"/>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F12" s="35"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F13" s="35"/>
+      <c r="F13" s="32"/>
     </row>
     <row r="14" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F14" s="35"/>
+      <c r="F14" s="32"/>
     </row>
     <row r="15" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F15" s="35"/>
+      <c r="F15" s="32"/>
     </row>
     <row r="16" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F16" s="35"/>
+      <c r="F16" s="32"/>
     </row>
     <row r="17" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F17" s="35"/>
+      <c r="F17" s="32"/>
     </row>
     <row r="18" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F18" s="35"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F19" s="35"/>
+      <c r="F19" s="32"/>
     </row>
     <row r="20" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F20" s="35"/>
+      <c r="F20" s="32"/>
     </row>
     <row r="21" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F21" s="35"/>
+      <c r="F21" s="32"/>
     </row>
     <row r="22" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F22" s="35"/>
+      <c r="F22" s="32"/>
     </row>
     <row r="23" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F23" s="35"/>
+      <c r="F23" s="32"/>
     </row>
     <row r="24" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F24" s="35"/>
+      <c r="F24" s="32"/>
     </row>
     <row r="25" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F25" s="35"/>
+      <c r="F25" s="32"/>
     </row>
     <row r="26" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F26" s="35"/>
+      <c r="F26" s="32"/>
     </row>
     <row r="27" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F27" s="35"/>
+      <c r="F27" s="32"/>
     </row>
     <row r="28" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F28" s="35"/>
+      <c r="F28" s="32"/>
     </row>
     <row r="29" spans="6:6" x14ac:dyDescent="0.2">
-      <c r="F29" s="35"/>
+      <c r="F29" s="32"/>
     </row>
   </sheetData>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5368,19 +5339,19 @@
     <col min="2" max="2" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="2" t="s">
         <v>273</v>
       </c>
     </row>
@@ -5403,46 +5374,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="21" t="s">
+      <c r="B1" s="18" t="s">
         <v>274</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="17" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="20" t="s">
         <v>276</v>
       </c>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="C4" s="22" t="s">
+      <c r="C4" s="19" t="s">
         <v>277</v>
       </c>
     </row>
@@ -5460,16 +5431,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.140625" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
     <col min="3" max="3" width="37.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" customWidth="1"/>
-    <col min="6" max="6" width="10" customWidth="1"/>
-    <col min="7" max="7" width="20" customWidth="1"/>
-    <col min="8" max="8" width="43.42578125" customWidth="1"/>
-    <col min="9" max="9" width="27.85546875" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="20.140625" customWidth="1"/>
+    <col min="5" max="5" width="22.140625" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="47.5703125" customWidth="1"/>
+    <col min="9" max="9" width="89" customWidth="1"/>
+    <col min="10" max="10" width="72.85546875" customWidth="1"/>
+    <col min="11" max="11" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5503,7 +5474,7 @@
       <c r="J1" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="K1" s="21" t="s">
         <v>289</v>
       </c>
     </row>
@@ -5517,10 +5488,10 @@
       <c r="C2" s="2" t="s">
         <v>291</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="22">
         <v>465.8</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="22">
         <v>46.58</v>
       </c>
       <c r="F2" s="2">
@@ -5538,7 +5509,7 @@
       <c r="J2" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="23">
         <v>17149</v>
       </c>
     </row>
@@ -5563,54 +5534,55 @@
     <col min="6" max="6" width="12.5703125" customWidth="1"/>
     <col min="7" max="7" width="13" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" customWidth="1"/>
-    <col min="9" max="14" width="13" customWidth="1"/>
-    <col min="15" max="15" width="30.85546875" customWidth="1"/>
+    <col min="9" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="42.140625" customWidth="1"/>
+    <col min="14" max="15" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="24" t="s">
         <v>296</v>
       </c>
-      <c r="B1" s="28" t="s">
+      <c r="B1" s="25" t="s">
         <v>297</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="25" t="s">
         <v>298</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="25" t="s">
         <v>299</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="25" t="s">
         <v>300</v>
       </c>
-      <c r="F1" s="29" t="s">
+      <c r="F1" s="26" t="s">
         <v>301</v>
       </c>
-      <c r="G1" s="29" t="s">
+      <c r="G1" s="26" t="s">
         <v>302</v>
       </c>
-      <c r="H1" s="27" t="s">
+      <c r="H1" s="24" t="s">
         <v>303</v>
       </c>
-      <c r="I1" s="27" t="s">
+      <c r="I1" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="J1" s="27" t="s">
+      <c r="J1" s="24" t="s">
         <v>305</v>
       </c>
-      <c r="K1" s="27" t="s">
+      <c r="K1" s="24" t="s">
         <v>306</v>
       </c>
-      <c r="L1" s="27" t="s">
+      <c r="L1" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="M1" s="27" t="s">
+      <c r="M1" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="24" t="s">
         <v>309</v>
       </c>
-      <c r="O1" s="27" t="s">
+      <c r="O1" s="24" t="s">
         <v>310</v>
       </c>
     </row>
@@ -5621,41 +5593,41 @@
       <c r="B2" s="2" t="s">
         <v>311</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="27">
         <v>45717</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="28" t="s">
         <v>312</v>
       </c>
-      <c r="F2" s="32">
+      <c r="F2" s="29">
         <v>0</v>
       </c>
-      <c r="G2" s="32">
+      <c r="G2" s="29">
         <v>0</v>
       </c>
-      <c r="H2" s="33" t="s">
+      <c r="H2" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="I2" s="33" t="s">
+      <c r="I2" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="L2" s="33" t="s">
+      <c r="L2" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="M2" s="33" t="s">
+      <c r="M2" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="N2" s="34" t="s">
+      <c r="N2" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="O2" s="34" t="s">
+      <c r="O2" s="31" t="s">
         <v>314</v>
       </c>
     </row>

</xml_diff>